<commit_message>
format fix header table
</commit_message>
<xml_diff>
--- a/report/excel/report.xlsx
+++ b/report/excel/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="161">
   <si>
     <t>รายงานการเดินทางประจำวัน</t>
   </si>
@@ -49,211 +49,457 @@
     <t>ตำแหน่งสิ้นสุด</t>
   </si>
   <si>
-    <t>2019-09-26 02:32:03</t>
-  </si>
-  <si>
-    <t>2019-09-26 02:38:15</t>
-  </si>
-  <si>
-    <t>6 นาที</t>
-  </si>
-  <si>
-    <t>17.980230000000002,100.0892</t>
-  </si>
-  <si>
-    <t>17.97994,100.08992</t>
-  </si>
-  <si>
-    <t>2019-09-26 03:47:36</t>
-  </si>
-  <si>
-    <t>2019-09-26 03:47:54</t>
+    <t>2019-12-11 01:16:51</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:19:37</t>
+  </si>
+  <si>
+    <t>2 นาที</t>
+  </si>
+  <si>
+    <t>18.625015,99.049165</t>
+  </si>
+  <si>
+    <t>18.625213,99.050056</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:19:42</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:19:45</t>
   </si>
   <si>
     <t>0 นาที</t>
   </si>
   <si>
-    <t>17.98002,100.08973</t>
-  </si>
-  <si>
-    <t>2019-09-26 03:48:40</t>
-  </si>
-  <si>
-    <t>2019-09-26 03:57:55</t>
+    <t>18.6252,99.050056</t>
+  </si>
+  <si>
+    <t>18.625201,99.050056</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:19:46</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:19:49</t>
+  </si>
+  <si>
+    <t>18.625206,99.050056</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:20:00</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:20:03</t>
+  </si>
+  <si>
+    <t>18.625236,99.050066</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:20:05</t>
+  </si>
+  <si>
+    <t>18.625236,99.050068</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:23:58</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:24:08</t>
+  </si>
+  <si>
+    <t>18.625403,99.050071</t>
+  </si>
+  <si>
+    <t>18.625413,99.050076</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:24:10</t>
+  </si>
+  <si>
+    <t>18.62538,99.050068</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:24:11</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:24:13</t>
+  </si>
+  <si>
+    <t>18.625358,99.050068</t>
+  </si>
+  <si>
+    <t>18.625348,99.050068</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:25:03</t>
+  </si>
+  <si>
+    <t>2019-12-11 01:25:21</t>
+  </si>
+  <si>
+    <t>18.625281,99.050036</t>
+  </si>
+  <si>
+    <t>18.625273,99.050033</t>
+  </si>
+  <si>
+    <t>2019-12-11 02:27:38</t>
+  </si>
+  <si>
+    <t>2019-12-11 02:55:53</t>
+  </si>
+  <si>
+    <t>28 นาที</t>
+  </si>
+  <si>
+    <t>18.625321,99.049918</t>
+  </si>
+  <si>
+    <t>18.741873,98.959943</t>
+  </si>
+  <si>
+    <t>2019-12-11 02:55:58</t>
+  </si>
+  <si>
+    <t>2019-12-11 02:56:00</t>
+  </si>
+  <si>
+    <t>18.741858,98.959935</t>
+  </si>
+  <si>
+    <t>2019-12-11 02:56:07</t>
+  </si>
+  <si>
+    <t>2019-12-11 02:56:09</t>
+  </si>
+  <si>
+    <t>18.74186,98.959938</t>
+  </si>
+  <si>
+    <t>2019-12-11 04:02:29</t>
+  </si>
+  <si>
+    <t>2019-12-11 04:24:31</t>
+  </si>
+  <si>
+    <t>22 นาที</t>
+  </si>
+  <si>
+    <t>18.741823,98.959955</t>
+  </si>
+  <si>
+    <t>18.786466,98.982768</t>
+  </si>
+  <si>
+    <t>2019-12-11 04:45:15</t>
+  </si>
+  <si>
+    <t>2019-12-11 05:17:56</t>
+  </si>
+  <si>
+    <t>32 นาที</t>
+  </si>
+  <si>
+    <t>18.786078,98.982675</t>
+  </si>
+  <si>
+    <t>18.625191,99.050005</t>
+  </si>
+  <si>
+    <t>2019-12-11 07:02:12</t>
+  </si>
+  <si>
+    <t>2019-12-11 07:12:22</t>
+  </si>
+  <si>
+    <t>10 นาที</t>
+  </si>
+  <si>
+    <t>18.625378,99.050036</t>
+  </si>
+  <si>
+    <t>18.629673,99.049201</t>
+  </si>
+  <si>
+    <t>2019-12-11 07:16:01</t>
+  </si>
+  <si>
+    <t>2019-12-11 08:01:32</t>
+  </si>
+  <si>
+    <t>45 นาที</t>
+  </si>
+  <si>
+    <t>18.629955,99.049303</t>
+  </si>
+  <si>
+    <t>18.786121,98.982503</t>
+  </si>
+  <si>
+    <t>2019-12-11 09:40:22</t>
+  </si>
+  <si>
+    <t>2019-12-11 09:52:11</t>
+  </si>
+  <si>
+    <t>11 นาที</t>
+  </si>
+  <si>
+    <t>18.786418,98.984091</t>
+  </si>
+  <si>
+    <t>18.780811,98.97663</t>
+  </si>
+  <si>
+    <t>2019-12-11 11:57:33</t>
+  </si>
+  <si>
+    <t>2019-12-11 12:07:21</t>
   </si>
   <si>
     <t>9 นาที</t>
   </si>
   <si>
-    <t>2019-09-26 03:58:40</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:07:55</t>
-  </si>
-  <si>
-    <t>18.02537,100.11095999999999</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:08:40</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:17:55</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:18:40</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:27:55</t>
-  </si>
-  <si>
-    <t>18.12795,100.16852999999999</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:28:42</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:37:55</t>
-  </si>
-  <si>
-    <t>18.210089999999997,100.19924</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:38:15</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:48:01</t>
-  </si>
-  <si>
-    <t>18.22192,100.198</t>
-  </si>
-  <si>
-    <t>18.291439999999998,100.25655</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:48:41</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:57:55</t>
-  </si>
-  <si>
-    <t>18.332189999999997,100.27435</t>
-  </si>
-  <si>
-    <t>2019-09-26 04:58:41</t>
-  </si>
-  <si>
-    <t>2019-09-26 05:07:55</t>
-  </si>
-  <si>
-    <t>18.385389999999997,100.19604000000001</t>
-  </si>
-  <si>
-    <t>2019-09-26 05:08:40</t>
-  </si>
-  <si>
-    <t>2019-09-26 05:17:55</t>
-  </si>
-  <si>
-    <t>18.46121,100.1395</t>
-  </si>
-  <si>
-    <t>2019-09-26 05:18:39</t>
-  </si>
-  <si>
-    <t>2019-09-26 05:27:55</t>
-  </si>
-  <si>
-    <t>18.499789999999997,100.13306</t>
-  </si>
-  <si>
-    <t>2019-09-26 05:28:40</t>
-  </si>
-  <si>
-    <t>2019-09-26 07:34:59</t>
-  </si>
-  <si>
-    <t>2 ชั่วโมง 6 นาที</t>
-  </si>
-  <si>
-    <t>19.16702,99.90683</t>
-  </si>
-  <si>
-    <t>2019-09-26 16:36:51</t>
-  </si>
-  <si>
-    <t>2019-09-26 16:38:37</t>
+    <t>18.780848,98.976651</t>
+  </si>
+  <si>
+    <t>18.786085,98.982805</t>
+  </si>
+  <si>
+    <t>2019-12-11 12:21:47</t>
+  </si>
+  <si>
+    <t>2019-12-11 12:46:56</t>
+  </si>
+  <si>
+    <t>25 นาที</t>
+  </si>
+  <si>
+    <t>18.784965,98.982163</t>
+  </si>
+  <si>
+    <t>18.741845,98.959481</t>
+  </si>
+  <si>
+    <t>2019-12-11 13:55:39</t>
+  </si>
+  <si>
+    <t>2019-12-11 14:15:28</t>
+  </si>
+  <si>
+    <t>19 นาที</t>
+  </si>
+  <si>
+    <t>18.741766,98.959483</t>
+  </si>
+  <si>
+    <t>18.713116,99.037063</t>
+  </si>
+  <si>
+    <t>2019-12-11 14:22:16</t>
+  </si>
+  <si>
+    <t>2019-12-11 14:39:52</t>
+  </si>
+  <si>
+    <t>17 นาที</t>
+  </si>
+  <si>
+    <t>18.713151,99.037051</t>
+  </si>
+  <si>
+    <t>18.625215,99.049773</t>
+  </si>
+  <si>
+    <t>2019-12-11 14:55:54</t>
+  </si>
+  <si>
+    <t>2019-12-11 14:57:33</t>
   </si>
   <si>
     <t>1 นาที</t>
   </si>
   <si>
-    <t>19.189510000000002,99.87925999999999</t>
-  </si>
-  <si>
-    <t>2019-09-26 17:05:49</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:01:10</t>
-  </si>
-  <si>
-    <t>2 ชั่วโมง 55 นาที</t>
-  </si>
-  <si>
-    <t>19.189510000000002,99.87925</t>
-  </si>
-  <si>
-    <t>18.098380000000002,100.1328</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:02:04</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:11:10</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:12:04</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:19:07</t>
-  </si>
-  <si>
-    <t>7 นาที</t>
-  </si>
-  <si>
-    <t>17.97947,100.09048</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:38:50</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:39:41</t>
-  </si>
-  <si>
-    <t>17.97975,100.08974</t>
-  </si>
-  <si>
-    <t>17.97998,100.08968</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:40:00</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:42:39</t>
-  </si>
-  <si>
-    <t>2 นาที</t>
-  </si>
-  <si>
-    <t>17.98063,100.08932</t>
-  </si>
-  <si>
-    <t>17.98088,100.08943</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:43:33</t>
-  </si>
-  <si>
-    <t>2019-09-26 20:44:50</t>
+    <t>18.625458,99.049853</t>
+  </si>
+  <si>
+    <t>18.625731,99.049128</t>
+  </si>
+  <si>
+    <t>2019-12-11 15:11:02</t>
+  </si>
+  <si>
+    <t>2019-12-11 15:41:37</t>
+  </si>
+  <si>
+    <t>30 นาที</t>
+  </si>
+  <si>
+    <t>18.625725,99.049125</t>
+  </si>
+  <si>
+    <t>18.786213,98.982411</t>
+  </si>
+  <si>
+    <t>2019-12-11 16:43:39</t>
+  </si>
+  <si>
+    <t>2019-12-11 16:53:14</t>
+  </si>
+  <si>
+    <t>18.780261,98.976668</t>
+  </si>
+  <si>
+    <t>2019-12-11 17:34:14</t>
+  </si>
+  <si>
+    <t>2019-12-11 18:17:07</t>
+  </si>
+  <si>
+    <t>42 นาที</t>
+  </si>
+  <si>
+    <t>18.780221,98.976695</t>
+  </si>
+  <si>
+    <t>18.625403,99.04964</t>
+  </si>
+  <si>
+    <t>2019-12-11 19:26:01</t>
+  </si>
+  <si>
+    <t>2019-12-11 19:27:28</t>
+  </si>
+  <si>
+    <t>18.625383,99.049816</t>
+  </si>
+  <si>
+    <t>18.625338,99.049805</t>
+  </si>
+  <si>
+    <t>2019-12-11 19:41:40</t>
+  </si>
+  <si>
+    <t>2019-12-11 19:42:59</t>
+  </si>
+  <si>
+    <t>18.625395,99.049868</t>
+  </si>
+  <si>
+    <t>18.62497,99.049206</t>
+  </si>
+  <si>
+    <t>2019-12-11 23:23:12</t>
+  </si>
+  <si>
+    <t>2019-12-11 23:26:02</t>
+  </si>
+  <si>
+    <t>18.624851,99.0493</t>
+  </si>
+  <si>
+    <t>18.625345,99.049853</t>
+  </si>
+  <si>
+    <t>2019-12-11 23:43:53</t>
+  </si>
+  <si>
+    <t>2019-12-11 23:45:30</t>
+  </si>
+  <si>
+    <t>18.625393,99.049885</t>
+  </si>
+  <si>
+    <t>18.625191,99.05002</t>
+  </si>
+  <si>
+    <t>2019-12-12 01:34:04</t>
+  </si>
+  <si>
+    <t>2019-12-12 02:03:12</t>
+  </si>
+  <si>
+    <t>29 นาที</t>
+  </si>
+  <si>
+    <t>18.625268,99.049971</t>
+  </si>
+  <si>
+    <t>18.7419,98.959901</t>
+  </si>
+  <si>
+    <t>2019-12-12 02:20:34</t>
+  </si>
+  <si>
+    <t>2019-12-12 02:41:50</t>
+  </si>
+  <si>
+    <t>21 นาที</t>
+  </si>
+  <si>
+    <t>18.741848,98.959938</t>
+  </si>
+  <si>
+    <t>18.786403,98.982635</t>
+  </si>
+  <si>
+    <t>2019-12-12 03:05:52</t>
+  </si>
+  <si>
+    <t>2019-12-12 03:40:14</t>
+  </si>
+  <si>
+    <t>34 นาที</t>
+  </si>
+  <si>
+    <t>18.786188,98.98255</t>
+  </si>
+  <si>
+    <t>18.62523,99.05</t>
+  </si>
+  <si>
+    <t>2019-12-12 06:56:06</t>
+  </si>
+  <si>
+    <t>2019-12-12 06:58:36</t>
+  </si>
+  <si>
+    <t>18.625443,99.049911</t>
+  </si>
+  <si>
+    <t>18.6255,99.04952</t>
+  </si>
+  <si>
+    <t>2019-12-12 07:04:25</t>
+  </si>
+  <si>
+    <t>2019-12-12 07:48:25</t>
+  </si>
+  <si>
+    <t>44 นาที</t>
+  </si>
+  <si>
+    <t>18.625798,99.048891</t>
+  </si>
+  <si>
+    <t>18.786466,98.982725</t>
+  </si>
+  <si>
+    <t>2019-12-12 09:19:10</t>
+  </si>
+  <si>
+    <t>2019-12-12 09:27:11</t>
+  </si>
+  <si>
+    <t>8 นาที</t>
+  </si>
+  <si>
+    <t>18.785378,98.98207</t>
+  </si>
+  <si>
+    <t>18.7806,98.976666</t>
   </si>
 </sst>
 </file>
@@ -630,10 +876,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A24" sqref="A24:H24"/>
+      <selection activeCell="A39" sqref="A39:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -710,13 +956,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D5" s="5">
-        <v>0.08</v>
+        <v>0.22</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>7.18</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>12</v>
@@ -751,15 +997,15 @@
         <v>18</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -771,455 +1017,845 @@
         <v>0</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5">
-        <v>5.64</v>
+        <v>0</v>
       </c>
       <c r="E8" s="5">
-        <v>15.67</v>
+        <v>0</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="5">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="D9" s="5">
         <v>0</v>
       </c>
       <c r="E9" s="5">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5">
-        <v>13.69</v>
+        <v>0</v>
       </c>
       <c r="E10" s="5">
-        <v>52.46</v>
+        <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="5">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="D11" s="5">
-        <v>9.69</v>
+        <v>0</v>
       </c>
       <c r="E11" s="5">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="5">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="D12" s="5">
-        <v>10.01</v>
+        <v>0</v>
       </c>
       <c r="E12" s="5">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="5">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="D13" s="5">
-        <v>7.54</v>
+        <v>0</v>
       </c>
       <c r="E13" s="5">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D14" s="5">
-        <v>10.16</v>
+        <v>23.49</v>
       </c>
       <c r="E14" s="5">
-        <v>61</v>
+        <v>57.25</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="D15" s="5">
-        <v>10.33</v>
+        <v>0</v>
       </c>
       <c r="E15" s="5">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C16" s="5">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="D16" s="5">
-        <v>4.34</v>
+        <v>0</v>
       </c>
       <c r="E16" s="5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C17" s="5">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D17" s="5">
-        <v>85.4</v>
+        <v>9.01</v>
       </c>
       <c r="E17" s="5">
-        <v>66</v>
+        <v>36.8</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C18" s="5">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D18" s="5">
-        <v>0</v>
+        <v>25.81</v>
       </c>
       <c r="E18" s="5">
-        <v>0</v>
+        <v>62.6</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C19" s="5">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D19" s="5">
-        <v>136.88</v>
+        <v>1.21</v>
       </c>
       <c r="E19" s="5">
-        <v>51.62</v>
+        <v>16.95</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="5">
         <v>62</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="5">
-        <v>73</v>
-      </c>
       <c r="D20" s="5">
-        <v>0</v>
+        <v>24.81</v>
       </c>
       <c r="E20" s="5">
-        <v>73</v>
+        <v>58.98</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="5" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C21" s="5">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="D21" s="5">
-        <v>15.37</v>
+        <v>2.52</v>
       </c>
       <c r="E21" s="5">
-        <v>58.24</v>
+        <v>18.36</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C22" s="5">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D22" s="5">
-        <v>0.03</v>
+        <v>2.12</v>
       </c>
       <c r="E22" s="5">
-        <v>2.67</v>
+        <v>16.45</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="5" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C23" s="5">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D23" s="5">
-        <v>0.03</v>
+        <v>7.15</v>
       </c>
       <c r="E23" s="5">
-        <v>9</v>
+        <v>35.29</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C24" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>13.46</v>
       </c>
       <c r="E24" s="5">
-        <v>0</v>
+        <v>53.76</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>76</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="5">
+        <v>74</v>
+      </c>
+      <c r="D25" s="5">
+        <v>12.82</v>
+      </c>
+      <c r="E25" s="5">
+        <v>52.19</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="E26" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="5">
+        <v>44</v>
+      </c>
+      <c r="D27" s="5">
+        <v>25.58</v>
+      </c>
+      <c r="E27" s="5">
+        <v>40.67</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="5">
+        <v>32</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2.32</v>
+      </c>
+      <c r="E28" s="5">
+        <v>26.46</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="5">
+        <v>67</v>
+      </c>
+      <c r="D29" s="5">
+        <v>25.9</v>
+      </c>
+      <c r="E29" s="5">
+        <v>51.89</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="5">
+        <v>10</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0.17</v>
+      </c>
+      <c r="E31" s="5">
+        <v>8.29</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.17</v>
+      </c>
+      <c r="E32" s="5">
+        <v>3.93</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="5">
+        <v>8</v>
+      </c>
+      <c r="D33" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="E33" s="5">
+        <v>5.71</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="5">
+        <v>43</v>
+      </c>
+      <c r="D34" s="5">
+        <v>23.52</v>
+      </c>
+      <c r="E34" s="5">
+        <v>38.3</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="5">
+        <v>44</v>
+      </c>
+      <c r="D35" s="5">
+        <v>8.98</v>
+      </c>
+      <c r="E35" s="5">
+        <v>40.15</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="5">
+        <v>45</v>
+      </c>
+      <c r="D36" s="5">
+        <v>25.79</v>
+      </c>
+      <c r="E36" s="5">
+        <v>40.06</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="5">
+        <v>15</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="E37" s="5">
+        <v>4.78</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="5">
+        <v>95</v>
+      </c>
+      <c r="D38" s="5">
+        <v>25.58</v>
+      </c>
+      <c r="E38" s="5">
+        <v>76.29</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="5">
+        <v>33</v>
+      </c>
+      <c r="D39" s="5">
+        <v>2.39</v>
+      </c>
+      <c r="E39" s="5">
+        <v>28.09</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>